<commit_message>
Updated the course file
</commit_message>
<xml_diff>
--- a/Course Files/ToolsDescriptionsSP25_freya_junru.xlsx
+++ b/Course Files/ToolsDescriptionsSP25_freya_junru.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Freedomsongs/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Freedomsongs/Desktop/Write-Out-Loud/Course Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41DF0866-33CE-694C-9C8A-CED5B2ACCE83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A67B2926-93E3-CB41-A610-19CFA5A72261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12180" yWindow="760" windowWidth="31020" windowHeight="17660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3540" yWindow="760" windowWidth="31020" windowHeight="17660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -215,6 +215,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -226,9 +229,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -515,80 +515,81 @@
   </sheetPr>
   <dimension ref="A2:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="60.1640625" customWidth="1"/>
     <col min="2" max="2" width="66.33203125" customWidth="1"/>
+    <col min="5" max="7" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:2" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="8" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="8"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="9"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="8" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="8"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="9"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="8"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="8" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="73" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="8"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="9"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="89" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="8"/>
+      <c r="A12" s="7"/>
+      <c r="B12" s="9"/>
     </row>
     <row r="13" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
@@ -613,16 +614,16 @@
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="8" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="240" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="B17" s="8"/>
+      <c r="A17" s="7"/>
+      <c r="B17" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="12">

</xml_diff>